<commit_message>
Added link in CodeExcel.xlsx
</commit_message>
<xml_diff>
--- a/CodeExcel.xlsx
+++ b/CodeExcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\44691\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S530473\Desktop\GDP1\Project-Charter-Group-D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{715E28C0-66D4-4F8E-9AB9-358701F362B1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{480C9374-DB6A-42E7-A9B2-A81BBF843A57}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{B22338A6-5A6F-4A97-976D-53EBE18763A7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{B22338A6-5A6F-4A97-976D-53EBE18763A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Codeword" sheetId="1" r:id="rId1"/>
@@ -320,7 +320,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,6 +355,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -373,10 +381,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -388,8 +397,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -704,9 +715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B97F6B-761F-4606-AB72-71E475E30B14}">
   <dimension ref="A1:P96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1653,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC864E5D-1E68-4688-80C9-938D9F9D4B08}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1668,11 +1677,14 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>93</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" location="Codeword!A1" display="Hoot 96" xr:uid="{28A0BBA9-CD2D-4FBE-82E9-9F6C3F4AE3B5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>